<commit_message>
Update Azure Network Documentation Template.xlsx
</commit_message>
<xml_diff>
--- a/learning_path_modules/04_ALZ_Accelerator/sources/Azure Network Documentation Template.xlsx
+++ b/learning_path_modules/04_ALZ_Accelerator/sources/Azure Network Documentation Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25707"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/jovella_microsoft_com/Documents/Git/what-the-caf/learning_path_modules/04_ALZ_Accelerator/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{E489F088-6B2F-471E-B231-1A059A82CF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EE6471C-4B26-46FB-91EC-DF24918A56FF}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{E489F088-6B2F-471E-B231-1A059A82CF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC0B68A3-C3A0-4F04-98CE-7092E334B80D}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C820F456-7308-4348-96BC-0FE680A270E1}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{C820F456-7308-4348-96BC-0FE680A270E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Subnet Name</t>
   </si>
@@ -68,12 +68,6 @@
     <t>UDR</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Documentation</t>
   </si>
   <si>
@@ -87,6 +81,9 @@
   </si>
   <si>
     <t>AzureBastion</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -466,22 +463,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3A99E0-BDF6-4077-AD11-335A99E92C0A}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="198" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.29296875" customWidth="1"/>
+    <col min="2" max="2" width="19.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1171875" customWidth="1"/>
+    <col min="4" max="4" width="20.703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -504,10 +501,10 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -515,25 +512,25 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -541,10 +538,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -552,7 +549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -560,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
february 2023 content update
</commit_message>
<xml_diff>
--- a/learning_path_modules/04_ALZ_Accelerator/sources/Azure Network Documentation Template.xlsx
+++ b/learning_path_modules/04_ALZ_Accelerator/sources/Azure Network Documentation Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26125"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -456,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3A99E0-BDF6-4077-AD11-335A99E92C0A}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="198" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="198" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>